<commit_message>
add properties for EPolygon in QStudioSCADA and QSCADARunTime.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -466,7 +466,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -504,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
@@ -512,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add properties for EEllipse in QStudioSCADA and QSCADARunTime.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="28035" windowHeight="12345"/>
@@ -73,8 +73,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,12 +91,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -113,12 +131,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -126,7 +153,7 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -177,7 +204,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -251,7 +278,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -286,7 +312,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -462,20 +487,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="45.25" customWidth="1"/>
     <col min="2" max="2" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,173 +508,173 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:1">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:1">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:1">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:1">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:1">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:1">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:1">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:1">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:1">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:1">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:1">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:1">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:1">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:1">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:1">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:1">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:1">
       <c r="A39" s="1"/>
     </row>
   </sheetData>
@@ -660,19 +685,20 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -680,12 +706,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add properties for ELine in QStudioSCADA and QSCADARunTime.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="28035" windowHeight="12345"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -184,11 +185,6 @@
       <tableStyleElement type="headerRow" dxfId="1"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -491,7 +487,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -544,16 +540,16 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>

<commit_message>
add properties for EArrow in QStudioSCADA and QSCADARunTime.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -487,7 +486,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -548,16 +547,16 @@
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2">

</xml_diff>

<commit_message>
add properties for ERect in QStudioSCADA and QSCADARunTime.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -486,7 +486,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -555,16 +555,16 @@
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2">

</xml_diff>

<commit_message>
add properties for EPicture in QStudioSCADA and QSCADARunTime.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -486,7 +486,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -563,16 +563,16 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2">

</xml_diff>

<commit_message>
add properties for EPushButton in QStudioSCADA and QSCADARunTime.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="28035" windowHeight="12345"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="28035" windowHeight="12345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="画面编辑器" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="事件功能" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>功能模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,13 +68,67 @@
   <si>
     <t>文本标签</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>切换画面</t>
+  </si>
+  <si>
+    <t>返回画面</t>
+  </si>
+  <si>
+    <t>设置时间</t>
+  </si>
+  <si>
+    <t>执行脚本</t>
+  </si>
+  <si>
+    <t>设置变量值</t>
+  </si>
+  <si>
+    <t>获取变量的值</t>
+  </si>
+  <si>
+    <t>切换变量状态</t>
+  </si>
+  <si>
+    <t>设置系统变量值</t>
+  </si>
+  <si>
+    <t>获取系统变量值</t>
+  </si>
+  <si>
+    <t>变量值自增</t>
+  </si>
+  <si>
+    <t>变量值自减</t>
+  </si>
+  <si>
+    <t>隐藏控件</t>
+  </si>
+  <si>
+    <t>显示控件</t>
+  </si>
+  <si>
+    <t>失效控件</t>
+  </si>
+  <si>
+    <t>生效控件</t>
+  </si>
+  <si>
+    <t>偏移控件</t>
+  </si>
+  <si>
+    <t>闪烁控件</t>
+  </si>
+  <si>
+    <t>停止闪烁</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -125,13 +179,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -145,6 +247,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -153,7 +273,7 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -184,6 +304,11 @@
       <tableStyleElement type="headerRow" dxfId="1"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -199,7 +324,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -273,6 +398,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -307,6 +433,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -482,20 +609,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="A2:B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="45.25" customWidth="1"/>
     <col min="2" max="2" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -511,7 +638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -519,7 +646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -527,7 +654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -535,7 +662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -543,7 +670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -551,7 +678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -559,7 +686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -567,23 +694,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -591,85 +718,85 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
     </row>
   </sheetData>
@@ -688,25 +815,281 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="28.25" customWidth="1"/>
+    <col min="2" max="2" width="26.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" s="5"/>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" s="5"/>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" s="5"/>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" s="5"/>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" s="5"/>
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" s="5"/>
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" s="5"/>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" s="5"/>
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" s="5"/>
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" s="5"/>
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" s="5"/>
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" s="5"/>
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" s="5"/>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" s="5"/>
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" s="5"/>
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" s="5"/>
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" s="5"/>
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" s="5"/>
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" s="5"/>
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" s="5"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" s="8"/>
+      <c r="B41" s="7"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" s="9"/>
+      <c r="B43" s="10"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B43">
+      <formula1>"未开始,已完成,进行中"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add properties for EInputEdit in QStudioSCADA and update ProjectManager's ui.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="28035" windowHeight="12345" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="28035" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="画面编辑器" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>功能模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>输入编辑框</t>
-  </si>
-  <si>
-    <t>变量显示文本框</t>
   </si>
   <si>
     <t>已完成</t>
@@ -233,7 +230,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -244,9 +241,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -612,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="A2:B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -635,15 +629,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
@@ -651,7 +645,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
@@ -659,7 +653,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
@@ -667,7 +661,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
@@ -675,7 +669,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
@@ -683,7 +677,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
@@ -691,7 +685,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
@@ -699,7 +693,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
@@ -707,16 +701,11 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
@@ -818,7 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -829,248 +818,248 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="5" t="s">
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="5" t="s">
+      <c r="B13" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="5" t="s">
+      <c r="B16" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>13</v>
+      <c r="B18" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="5"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="5"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="5"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="6"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="5"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="5"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="6"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="5"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="5"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="5"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="6"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="5"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="6"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="5"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="6"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="5"/>
-      <c r="B29" s="7"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="6"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="5"/>
-      <c r="B30" s="7"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="6"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="5"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="6"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="5"/>
-      <c r="B32" s="7"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="6"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="5"/>
-      <c r="B33" s="7"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="6"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" s="5"/>
-      <c r="B34" s="7"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="6"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" s="5"/>
-      <c r="B35" s="7"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="6"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" s="5"/>
-      <c r="B36" s="7"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="6"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="5"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="6"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="5"/>
-      <c r="B38" s="7"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="6"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="6"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="6"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="8"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="6"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="6"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="9"/>
-      <c r="B43" s="10"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update develop guide document.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="28035" windowHeight="12345"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="28035" windowHeight="12345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="画面编辑器" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>功能模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>未开始</t>
-  </si>
-  <si>
-    <t>进行中</t>
   </si>
   <si>
     <t>文本标签</t>
@@ -142,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,12 +149,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,13 +231,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
@@ -259,6 +247,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -606,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -634,7 +625,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
@@ -700,8 +691,8 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
@@ -807,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -818,248 +809,248 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="4" t="s">
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="4" t="s">
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="4" t="s">
+      <c r="B16" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="4"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="4"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="4"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="4"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="4"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="4"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="4"/>
-      <c r="B26" s="6"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="4"/>
-      <c r="B27" s="6"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="4"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="4"/>
-      <c r="B29" s="6"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="4"/>
-      <c r="B30" s="6"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="4"/>
-      <c r="B31" s="6"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="4"/>
-      <c r="B32" s="6"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="4"/>
-      <c r="B33" s="6"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" s="4"/>
-      <c r="B34" s="6"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="5"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" s="4"/>
-      <c r="B35" s="6"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" s="4"/>
-      <c r="B36" s="6"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="4"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="4"/>
-      <c r="B38" s="6"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="7"/>
-      <c r="B39" s="6"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="7"/>
-      <c r="B40" s="6"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="7"/>
-      <c r="B41" s="6"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="7"/>
-      <c r="B42" s="6"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="8"/>
-      <c r="B43" s="9"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add class ElementIDHelper for element operate function.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>功能模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>设置时间</t>
-  </si>
-  <si>
-    <t>执行脚本</t>
   </si>
   <si>
     <t>设置变量值</t>
@@ -796,10 +793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -836,56 +833,56 @@
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
+      <c r="B4" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
+      <c r="B5" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
+      <c r="B6" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>12</v>
+      <c r="B7" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
+      <c r="B8" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>12</v>
+      <c r="B9" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>12</v>
+      <c r="B10" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
@@ -945,12 +942,8 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
@@ -1029,7 +1022,7 @@
       <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="3"/>
+      <c r="A38" s="6"/>
       <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
@@ -1045,17 +1038,13 @@
       <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="6"/>
-      <c r="B42" s="5"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="7"/>
-      <c r="B43" s="8"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B42">
       <formula1>"未开始,已完成,进行中"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add function showControlElement hideControlElement.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -796,7 +796,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -889,16 +889,16 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>12</v>
+      <c r="B11" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>12</v>
+      <c r="B12" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add enable/disableElement, moveElement, blinkElement function.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="28035" windowHeight="12345" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="事件功能" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>功能模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,9 +57,6 @@
     <t>已完成</t>
   </si>
   <si>
-    <t>未开始</t>
-  </si>
-  <si>
     <t>文本标签</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -106,20 +103,21 @@
     <t>生效控件</t>
   </si>
   <si>
+    <t>闪烁控件</t>
+  </si>
+  <si>
+    <t>停止闪烁</t>
+  </si>
+  <si>
     <t>偏移控件</t>
-  </si>
-  <si>
-    <t>闪烁控件</t>
-  </si>
-  <si>
-    <t>停止闪烁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,12 +144,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -231,9 +223,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -249,13 +238,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -306,7 +298,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -380,7 +372,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -415,7 +406,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -591,20 +581,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="45.25" customWidth="1"/>
     <col min="2" max="2" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -620,15 +610,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -636,7 +626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -644,7 +634,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -652,7 +642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -660,7 +650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -668,7 +658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -676,7 +666,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -684,7 +674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -692,88 +682,88 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:1">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:1">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:1">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:1">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:1">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:1">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:1">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:1">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:1">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:1">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:1">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:1">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:1">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:1">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:1">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:1">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:1">
       <c r="A39" s="1"/>
     </row>
   </sheetData>
@@ -792,254 +782,254 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="28.25" customWidth="1"/>
     <col min="2" max="2" width="26.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="3" t="s">
+      <c r="B11" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
+      <c r="B12" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="3" t="s">
+      <c r="B13" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="3" t="s">
+      <c r="B16" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B17" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="3"/>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="3"/>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="3"/>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="3"/>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="3"/>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="3"/>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="3"/>
-      <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="3"/>
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="3"/>
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="3"/>
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="3"/>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="3"/>
-      <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="3"/>
-      <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="3"/>
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B32" s="4"/>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="3"/>
-      <c r="B33" s="5"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="3"/>
-      <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="3"/>
-      <c r="B35" s="5"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="3"/>
-      <c r="B36" s="5"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="3"/>
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="6"/>
-      <c r="B38" s="5"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="6"/>
-      <c r="B39" s="5"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="6"/>
-      <c r="B40" s="5"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="6"/>
-      <c r="B41" s="5"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="7"/>
-      <c r="B42" s="8"/>
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="5"/>
+      <c r="B38" s="4"/>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="5"/>
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="5"/>
+      <c r="B40" s="4"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="5"/>
+      <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1053,12 +1043,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add element EIndicationLamp for QSCADARuntime.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QStudioSCADA\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="28035" windowHeight="12345"/>
   </bookViews>
@@ -317,6 +322,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -333,7 +341,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -375,7 +383,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,7 +418,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -622,7 +630,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -723,8 +731,8 @@
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>35</v>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add ESwitchButton for QSCADARunTime
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -630,7 +630,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -739,8 +739,8 @@
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>35</v>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add EMovingText in QStudioSCADA.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>功能模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -141,6 +141,9 @@
   <si>
     <t>进行中</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进行中</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -771,15 +774,15 @@
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>35</v>
+      <c r="B16" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add element EValueStick to QStudioSCADA.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
   <si>
     <t>功能模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -130,9 +130,6 @@
   <si>
     <t>移动文本</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>未开始</t>
   </si>
   <si>
     <t>时钟</t>
@@ -163,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,12 +170,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,7 +242,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -283,9 +274,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -754,8 +742,8 @@
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>37</v>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
@@ -763,7 +751,7 @@
         <v>33</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
@@ -776,7 +764,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
add element EJarShape to QStudioSCADA.
</commit_message>
<xml_diff>
--- a/doc/开发进度.xlsx
+++ b/doc/开发进度.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>功能模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -134,9 +134,6 @@
   <si>
     <t>时钟</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>进行中</t>
   </si>
 </sst>
 </file>
@@ -160,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,12 +167,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,7 +233,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -272,9 +263,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,7 +613,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -750,8 +738,8 @@
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>36</v>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>